<commit_message>
增加了一些新的字段需求，标注为红色，具体制作的时候需沟通 doc\table\Buff表.xlsx doc\table\Npc表.xlsx doc\table\人物等级表.xlsx doc\table\任务表.xlsx doc\table\场景表.xlsx doc\table\技能表.xlsx doc\table\道具表.xlsx
</commit_message>
<xml_diff>
--- a/doc/table/Buff表.xlsx
+++ b/doc/table/Buff表.xlsx
@@ -11,12 +11,12 @@
     <sheet name="字段说明" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -93,6 +93,22 @@
   </si>
   <si>
     <t>等级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUFF时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUFF类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否计算战斗力</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -122,12 +138,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -142,8 +164,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -445,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -457,9 +480,11 @@
     <col min="2" max="2" width="5.25" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +497,20 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -486,8 +523,20 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -500,8 +549,20 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -514,8 +575,20 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -528,8 +601,20 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -542,8 +627,20 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -556,8 +653,20 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -570,8 +679,20 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -584,8 +705,20 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -598,8 +731,20 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -611,6 +756,18 @@
       </c>
       <c r="D11" t="s">
         <v>22</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>